<commit_message>
Uniandes 2023: nuevas ideas programa lenguaje
</commit_message>
<xml_diff>
--- a/Especial_Uniandes_2023/1. CV/data/supervision_pre_es.xlsx
+++ b/Especial_Uniandes_2023/1. CV/data/supervision_pre_es.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\Especial_Uniandes_2023\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\Especial_Uniandes_2023\1. CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932AA273-1F30-46F2-A44E-B5A66D98030A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9323CBE3-1F60-4C17-8A84-D285205DC066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4695" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="supervision" sheetId="1" r:id="rId1"/>
@@ -119,9 +119,6 @@
     <t>2015 - 2016</t>
   </si>
   <si>
-    <t>Desde 2017</t>
-  </si>
-  <si>
     <t xml:space="preserve">Natalia Elízabeth Moreno Buitrago y Juan Felipe Pérez Ariza </t>
   </si>
   <si>
@@ -213,6 +210,9 @@
   </si>
   <si>
     <t>Supervisión docente (Desde 2019)</t>
+  </si>
+  <si>
+    <t>Desde 2020</t>
   </si>
 </sst>
 </file>
@@ -1074,7 +1074,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="A4:XFD4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="58.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,16 +1108,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1126,7 +1126,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1135,7 +1135,7 @@
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1146,13 +1146,13 @@
         <v>2023</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1160,16 +1160,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1180,13 +1180,13 @@
         <v>20</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1203,7 +1203,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1214,13 +1214,13 @@
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1231,13 +1231,13 @@
         <v>21</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1248,13 +1248,13 @@
         <v>23</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1265,13 +1265,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1282,13 +1282,13 @@
         <v>24</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1305,7 +1305,7 @@
         <v>10</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1322,7 +1322,7 @@
         <v>10</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1339,7 +1339,7 @@
         <v>10</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1356,7 +1356,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1373,7 +1373,7 @@
         <v>10</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1390,7 +1390,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1407,7 +1407,7 @@
         <v>10</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1424,7 +1424,7 @@
         <v>10</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>